<commit_message>
Use vlucas/phpdotenv for keys
</commit_message>
<xml_diff>
--- a/public_html/app/storage/excel/Visit Log - Spring Semester 2015.xlsx
+++ b/public_html/app/storage/excel/Visit Log - Spring Semester 2015.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>Day</t>
   </si>
@@ -145,22 +145,25 @@
     <t>30</t>
   </si>
   <si>
+    <t>12:30</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
     <t>Tuesday</t>
   </si>
   <si>
-    <t>12:30</t>
+    <t>14:30</t>
+  </si>
+  <si>
+    <t>Dokollari</t>
+  </si>
+  <si>
+    <t>ITC4417</t>
   </si>
   <si>
     <t>pending</t>
-  </si>
-  <si>
-    <t>14:30</t>
-  </si>
-  <si>
-    <t>Dokollari</t>
-  </si>
-  <si>
-    <t>ITC4417</t>
   </si>
 </sst>
 </file>
@@ -197,7 +200,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +217,16 @@
         </stop>
         <stop position="1">
           <color rgb="e5412d"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="linear" degree="90">
+        <stop position="0">
+          <color rgb="3fa67a"/>
+        </stop>
+        <stop position="1">
+          <color rgb="3fa67a"/>
         </stop>
       </gradientFill>
     </fill>
@@ -260,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -280,6 +293,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -1703,10 +1722,10 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B3" s="5">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>19</v>
@@ -1715,7 +1734,7 @@
         <v>2015</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>21</v>
@@ -1748,7 +1767,7 @@
         <v>28</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>30</v>
@@ -1756,58 +1775,58 @@
       <c r="R3" s="6"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="5">
+      <c r="A4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="7">
         <v>27</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="7">
         <v>2015</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="7">
         <v>126198</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" s="5" t="s">
+      <c r="P4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="R4" s="6"/>
+      <c r="R4" s="8"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Force git to keep publict_html/app/storage/backups|excel
</commit_message>
<xml_diff>
--- a/public_html/app/storage/excel/Visit Log - Spring Semester 2015.xlsx
+++ b/public_html/app/storage/excel/Visit Log - Spring Semester 2015.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>Day</t>
   </si>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t>14:30</t>
-  </si>
-  <si>
-    <t>pending</t>
   </si>
 </sst>
 </file>
@@ -203,7 +200,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,16 +227,6 @@
         </stop>
         <stop position="1">
           <color rgb="3fa67a"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill type="linear" degree="90">
-        <stop position="0">
-          <color rgb="888888"/>
-        </stop>
-        <stop position="1">
-          <color rgb="888888"/>
         </stop>
       </gradientFill>
     </fill>
@@ -276,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -296,12 +283,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -1832,58 +1813,58 @@
       <c r="R4" s="6"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>27</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>2015</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5">
         <v>126198</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q5" s="7" t="s">
+      <c r="P5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="R5" s="8"/>
+      <c r="R5" s="6"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>